<commit_message>
Test Posting docs updated
</commit_message>
<xml_diff>
--- a/posting-docs.xlsx
+++ b/posting-docs.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="18380" tabRatio="500"/>
+    <workbookView xWindow="19200" yWindow="-20" windowWidth="19200" windowHeight="21060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="SchoolName" sheetId="2" r:id="rId1"/>
+    <sheet name="Fields" sheetId="1" r:id="rId2"/>
+    <sheet name="Copy" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,43 +21,170 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Header 1</t>
-  </si>
-  <si>
-    <t>Header 2</t>
-  </si>
-  <si>
-    <t>Header 3</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Row2</t>
-  </si>
-  <si>
-    <t>Row3</t>
-  </si>
-  <si>
-    <t>Row22</t>
-  </si>
-  <si>
-    <t>Row33</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+  <si>
+    <t>SchoolName</t>
+  </si>
+  <si>
+    <t>Test University</t>
+  </si>
+  <si>
+    <t>DisplayName</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>Colspan</t>
+  </si>
+  <si>
+    <t>InputType</t>
+  </si>
+  <si>
+    <t>InputName</t>
+  </si>
+  <si>
+    <t>MaxLength</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Dropdown</t>
+  </si>
+  <si>
+    <t>StateID</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>CityID</t>
+  </si>
+  <si>
+    <t>InputID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>NameID</t>
+  </si>
+  <si>
+    <t>Hidden1</t>
+  </si>
+  <si>
+    <t>Hidden</t>
+  </si>
+  <si>
+    <t>HiddenID</t>
+  </si>
+  <si>
+    <t>Hidden2</t>
+  </si>
+  <si>
+    <t>HiddenID2</t>
+  </si>
+  <si>
+    <t>Program Area</t>
+  </si>
+  <si>
+    <t>ProgramID</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>CommentsID</t>
+  </si>
+  <si>
+    <t>By checking this box, I consent to receive phone calls and/or text messages from Post University at the phone number(s) provided, which may include a wireless number, using automated technology, to discuss their educational services. Checking this box is required for a school to contact me, without obligation to attend their university. I understand that my information will be handled in accordance with this site's privacy policy.</t>
+  </si>
+  <si>
+    <t>contact_permission</t>
+  </si>
+  <si>
+    <t>leadid_tcpa_disclosure</t>
+  </si>
+  <si>
+    <t>Checkbox</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "&lt;p&gt;Lorem ipsum dolor sit amet, consectetur adipiscing elit.&lt;/p&gt;\n&lt;p&gt;Lorem ipsum dolor sit amet, consectetur adipiscing elit.&lt;/p&gt;",</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "This school is great.",</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> "By clicking Submit, I acknowledge that I may be contacted by email, text message and/or phone via automated means at the number provided above, including my wireless number, if provided, by a representative of NCU. I also understand that consent is not a condition of enrollment."</t>
+  </si>
+  <si>
+    <t>"CopyText"</t>
+  </si>
+  <si>
+    <t>"DisclaimerText"</t>
+  </si>
+  <si>
+    <t>"AdditionalText"</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>ZipID</t>
+  </si>
+  <si>
+    <t>StateInput</t>
+  </si>
+  <si>
+    <t>CityInput</t>
+  </si>
+  <si>
+    <t>NameInput</t>
+  </si>
+  <si>
+    <t>HiddenInput</t>
+  </si>
+  <si>
+    <t>CommentsInput</t>
+  </si>
+  <si>
+    <t>ZipInput</t>
+  </si>
+  <si>
+    <t>ProgramInput</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +207,61 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="25">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,45 +591,309 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Write copy to JSON file working
</commit_message>
<xml_diff>
--- a/posting-docs.xlsx
+++ b/posting-docs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SchoolName" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="53">
   <si>
     <t>SchoolName</t>
   </si>
@@ -50,6 +50,9 @@
     <t>Value</t>
   </si>
   <si>
+    <t>DropDownOptions</t>
+  </si>
+  <si>
     <t>StateInput</t>
   </si>
   <si>
@@ -140,22 +143,22 @@
     <t>Checkbox</t>
   </si>
   <si>
-    <t>"CopyText"</t>
-  </si>
-  <si>
-    <t>"DisclaimerText"</t>
-  </si>
-  <si>
-    <t>"AdditionalText"</t>
-  </si>
-  <si>
-    <t>"&lt;p&gt;Lorem ipsum dolor sit amet, consectetur adipiscing elit.&lt;/p&gt;\n&lt;p&gt;Lorem ipsum dolor sit amet, consectetur adipiscing elit.&lt;/p&gt;",</t>
-  </si>
-  <si>
-    <t>"This school is great.",</t>
-  </si>
-  <si>
-    <t>"By clicking Submit, I acknowledge that I may be contacted by email, text message and/or phone via automated means at the number provided above, including my wireless number, if provided, by a representative of NCU. I also understand that consent is not a condition of enrollment."</t>
+    <t>CopyText</t>
+  </si>
+  <si>
+    <t>DisclaimerText</t>
+  </si>
+  <si>
+    <t>AdditionalText</t>
+  </si>
+  <si>
+    <t>This is the copytext</t>
+  </si>
+  <si>
+    <t>This is the disclaimer Text</t>
+  </si>
+  <si>
+    <t>This is the additional Text</t>
   </si>
   <si>
     <t>New York</t>
@@ -249,11 +252,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -278,7 +277,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C53" activeCellId="0" sqref="C53"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -312,10 +311,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -323,7 +322,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.162962962963"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.9962962962963"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.66296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.5296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.66296296296296"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.83333333333333"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3333333333333"/>
@@ -356,152 +355,155 @@
       <c r="H1" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="I1" s="0" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="C5" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="C7" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="C8" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>500</v>
@@ -509,23 +511,23 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="C9" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>5</v>
@@ -533,23 +535,23 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="C10" s="0" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>2</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H10" s="0" t="n">
         <v>1</v>
@@ -573,8 +575,8 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -584,24 +586,24 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -622,8 +624,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -642,26 +644,26 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>